<commit_message>
who. lots of commits
</commit_message>
<xml_diff>
--- a/chapters/ch10/docs/ch10-overhaul.xlsx
+++ b/chapters/ch10/docs/ch10-overhaul.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
@@ -10,6 +10,9 @@
     <sheet name="Dashboard" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Dashboard!$A$2:$Q$53</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -152,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,6 +175,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -431,6 +440,8 @@
   <colors>
     <mruColors>
       <color rgb="FFC0504D"/>
+      <color rgb="FFF79646"/>
+      <color rgb="FF9BBB59"/>
     </mruColors>
   </colors>
 </styleSheet>
@@ -679,11 +690,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="2042983432"/>
-        <c:axId val="2077352872"/>
+        <c:axId val="2119730216"/>
+        <c:axId val="2119640568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2042983432"/>
+        <c:axId val="2119730216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,7 +703,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2077352872"/>
+        <c:crossAx val="2119640568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -700,7 +711,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2077352872"/>
+        <c:axId val="2119640568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -710,7 +721,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2042983432"/>
+        <c:crossAx val="2119730216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -738,6 +749,307 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Security Intelligence Trend</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0277749387286854"/>
+          <c:y val="0.0292504570383912"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="9BBB59"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$24:$Q$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$25:$Q$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>175.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Medium</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$24:$Q$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$26:$Q$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>350.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>350.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C0504D"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$24:$Q$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$27:$Q$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-25"/>
+        <c:axId val="2121488616"/>
+        <c:axId val="2121491672"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2121488616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121491672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2121491672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121488616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -868,11 +1180,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2077699960"/>
-        <c:axId val="2079694936"/>
+        <c:axId val="2121345592"/>
+        <c:axId val="2121348536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2077699960"/>
+        <c:axId val="2121345592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,7 +1193,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079694936"/>
+        <c:crossAx val="2121348536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -889,7 +1201,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079694936"/>
+        <c:axId val="2121348536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -899,7 +1211,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2077699960"/>
+        <c:crossAx val="2121345592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -921,7 +1233,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1071,11 +1383,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2075928424"/>
-        <c:axId val="2079327928"/>
+        <c:axId val="2121373624"/>
+        <c:axId val="2121378040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2075928424"/>
+        <c:axId val="2121373624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,7 +1396,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079327928"/>
+        <c:crossAx val="2121378040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1092,7 +1404,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079327928"/>
+        <c:axId val="2121378040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1102,7 +1414,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075928424"/>
+        <c:crossAx val="2121373624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1124,7 +1436,1305 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Security Intelligence Trend</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0179916885389327"/>
+          <c:y val="0.0324074074074074"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C0504D"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Med</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F79646"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="9BBB59"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:axId val="2114935256"/>
+        <c:axId val="2123797800"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2114935256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2123797800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2123797800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2114935256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Highest Concern Assets</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0127916158367528"/>
+          <c:y val="0.020125786163522"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Incidents</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$18:$R$18</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Asset Grp 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Asset Grp 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Asset Grp 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Asset Grp 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Asset Grp 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$19:$R$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$18:$R$18</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Asset Grp 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Asset Grp 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Asset Grp 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Asset Grp 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Asset Grp 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$20:$R$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Exposures</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C0504D"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$18:$R$18</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Asset Grp 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Asset Grp 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Asset Grp 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Asset Grp 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Asset Grp 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$21:$R$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:axId val="2120070840"/>
+        <c:axId val="2120006712"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2120070840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz" anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2120006712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2120006712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9525">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="2120070840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.531196894260084"/>
+          <c:y val="0.171752011390733"/>
+          <c:w val="0.433427938499331"/>
+          <c:h val="0.0875072478685262"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Attack Event Types</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0224501312335958"/>
+          <c:y val="0.037037037037037"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$M$33:$M$40</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>DoS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Exploit</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>High</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Trojan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hostile</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Leakage</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Recon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Unknown</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$33:$N$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2119789320"/>
+        <c:axId val="2063846184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2119789320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2063846184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2063846184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2119789320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Monitored Security Event Trend</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0103126616472211"/>
+          <c:y val="0.0175131348511383"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Security</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$R$32:$Z$32</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Dec</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$33:$Z$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>60000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>175000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>160000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2063600616"/>
+        <c:axId val="2063845160"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2063600616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2063845160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2063845160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2063600616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Events By Severity</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.000549807727522431"/>
+          <c:y val="0.0324072952419409"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C0504D"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Med</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F79646"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="9BBB59"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:axId val="-2129605960"/>
+        <c:axId val="-2129205752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2129605960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2129205752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2129205752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2129605960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1337,11 +2947,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="2077687352"/>
-        <c:axId val="2077464504"/>
+        <c:axId val="2119765592"/>
+        <c:axId val="2063853960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2077687352"/>
+        <c:axId val="2119765592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,7 +2960,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2077464504"/>
+        <c:crossAx val="2063853960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1358,7 +2968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2077464504"/>
+        <c:axId val="2063853960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1368,7 +2978,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2077687352"/>
+        <c:crossAx val="2119765592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1401,736 +3011,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Highest Concern Assets</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0127916158367528"/>
-          <c:y val="0.020125786163522"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$M$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Incidents</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$N$18:$R$18</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Asset Grp 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Asset Grp 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Asset Grp 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Asset Grp 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Asset Grp 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$N$19:$R$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>75.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$M$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Intel</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$N$18:$R$18</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Asset Grp 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Asset Grp 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Asset Grp 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Asset Grp 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Asset Grp 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$N$20:$R$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$M$21</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Exposures</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="C0504D"/>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$N$18:$R$18</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Asset Grp 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Asset Grp 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Asset Grp 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Asset Grp 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Asset Grp 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$N$21:$R$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="75"/>
-        <c:axId val="2077918760"/>
-        <c:axId val="2043253416"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2077918760"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr rot="0" vert="horz" anchor="t" anchorCtr="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2043253416"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2043253416"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9525">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="2077918760"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.531196894260084"/>
-          <c:y val="0.171752011390733"/>
-          <c:w val="0.433427938499331"/>
-          <c:h val="0.0875072478685262"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Attack Event Types</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0224501312335958"/>
-          <c:y val="0.037037037037037"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$M$33:$M$40</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>DoS</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Exploit</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>High</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Trojan</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Hostile</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Leakage</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Recon</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Unknown</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$N$33:$N$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2073105032"/>
-        <c:axId val="2073988328"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2073105032"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073988328"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2073988328"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073105032"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Monitored Security Event Trend</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0103126616472211"/>
-          <c:y val="0.0175131348511383"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$Q$33</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Security</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$R$32:$Z$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>May</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Jun</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Jul</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Aug</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sep</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Oct</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Nov</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Dec</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Jan</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$R$33:$Z$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>60000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>25000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>125000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>100000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>175000.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>160000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2078716648"/>
-        <c:axId val="2077742264"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="2078716648"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2077742264"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2077742264"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078716648"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2355,11 +3236,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="2079885464"/>
-        <c:axId val="2038675256"/>
+        <c:axId val="2107774168"/>
+        <c:axId val="2063653416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2079885464"/>
+        <c:axId val="2107774168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2368,7 +3249,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2038675256"/>
+        <c:crossAx val="2063653416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2376,7 +3257,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2038675256"/>
+        <c:axId val="2063653416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2386,13 +3267,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079885464"/>
+        <c:crossAx val="2107774168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2412,7 +3294,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2625,11 +3507,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="2077505128"/>
-        <c:axId val="2077508184"/>
+        <c:axId val="2121288456"/>
+        <c:axId val="2121291512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2077505128"/>
+        <c:axId val="2121288456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2638,7 +3520,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2077508184"/>
+        <c:crossAx val="2121291512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2646,7 +3528,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2077508184"/>
+        <c:axId val="2121291512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2656,7 +3538,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2077505128"/>
+        <c:crossAx val="2121288456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2669,6 +3551,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2688,7 +3571,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2948,11 +3831,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="2080122952"/>
-        <c:axId val="2079678280"/>
+        <c:axId val="2121321736"/>
+        <c:axId val="2121324744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2080122952"/>
+        <c:axId val="2121321736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2971,7 +3854,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2079678280"/>
+        <c:crossAx val="2121324744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2979,7 +3862,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079678280"/>
+        <c:axId val="2121324744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2994,7 +3877,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2080122952"/>
+        <c:crossAx val="2121321736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3030,320 +3913,20 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Security Intelligence Trend</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0277749387286854"/>
-          <c:y val="0.0292504570383912"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$M$25</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Low</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$N$24:$Q$24</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mar</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Apr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$N$25:$Q$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>175.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$M$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Medium</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$N$24:$Q$24</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mar</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Apr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$N$26:$Q$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>350.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>350.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>200.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$M$27</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>High</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$N$24:$Q$24</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mar</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Apr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$N$27:$Q$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="-25"/>
-        <c:axId val="2079442856"/>
-        <c:axId val="2079445912"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2079442856"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079445912"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2079445912"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079442856"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3366,20 +3949,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>776816</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>84328</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3394,24 +3977,24 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3426,24 +4009,24 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData fLocksWithSheet="0"/>
+    <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3462,20 +4045,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3487,6 +4070,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3672,6 +4287,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4005,7 +4650,7 @@
   <dimension ref="P31:Q31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4015,7 +4660,9 @@
       <c r="Q31" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="58" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -4030,7 +4677,7 @@
   <dimension ref="A1:Z40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>